<commit_message>
Descarga de archivo de busqueda completo
</commit_message>
<xml_diff>
--- a/public/enviar/funcionarios.xlsx
+++ b/public/enviar/funcionarios.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="202">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="238">
   <si>
     <t>FECHA</t>
   </si>
@@ -80,6 +80,9 @@
     <t>5:17 a.m.</t>
   </si>
   <si>
+    <t>2:34 p.m.</t>
+  </si>
+  <si>
     <t>MARITZA ZACIPA</t>
   </si>
   <si>
@@ -89,6 +92,9 @@
     <t>5:22 a.m.</t>
   </si>
   <si>
+    <t>2:42 p.m.</t>
+  </si>
+  <si>
     <t>ALEJANDRA PERLAZA</t>
   </si>
   <si>
@@ -116,6 +122,9 @@
     <t>5:28 a.m.</t>
   </si>
   <si>
+    <t>2:36 p.m.</t>
+  </si>
+  <si>
     <t>JHON CARLOS FIGUEREDO</t>
   </si>
   <si>
@@ -128,12 +137,18 @@
     <t>5:42 a.m.</t>
   </si>
   <si>
+    <t>2:33 p.m.</t>
+  </si>
+  <si>
     <t>QVJ 49B/ MOTO</t>
   </si>
   <si>
     <t>MARTA EDITH PACHON</t>
   </si>
   <si>
+    <t>2:39 p.m.</t>
+  </si>
+  <si>
     <t>REEMPLAZOS</t>
   </si>
   <si>
@@ -146,6 +161,9 @@
     <t>GESTIÓN EMPRESARIAL 6° - 11°</t>
   </si>
   <si>
+    <t>2:45 p.m.</t>
+  </si>
+  <si>
     <t>BICICLETA</t>
   </si>
   <si>
@@ -161,6 +179,9 @@
     <t>5:45 a.m.</t>
   </si>
   <si>
+    <t>2:32 p.m.</t>
+  </si>
+  <si>
     <t>CRISTINA PINZÓN</t>
   </si>
   <si>
@@ -185,6 +206,9 @@
     <t>5:46 a.m.</t>
   </si>
   <si>
+    <t>2:31 p.m.</t>
+  </si>
+  <si>
     <t>YENNY GÓMEZ</t>
   </si>
   <si>
@@ -194,6 +218,9 @@
     <t>5:47 a.m.</t>
   </si>
   <si>
+    <t>2:44 p.m.</t>
+  </si>
+  <si>
     <t>ZCP 63E/ MOTO</t>
   </si>
   <si>
@@ -215,6 +242,9 @@
     <t>5:50 a.m.</t>
   </si>
   <si>
+    <t>12:35 p.m.</t>
+  </si>
+  <si>
     <t>SEBASTIAN GUTIERREZ</t>
   </si>
   <si>
@@ -224,6 +254,9 @@
     <t>5:52 a.m.</t>
   </si>
   <si>
+    <t>2:38 p.m.</t>
+  </si>
+  <si>
     <t>DAMAR NARVÁEZ</t>
   </si>
   <si>
@@ -245,12 +278,18 @@
     <t>5:54 a.m.</t>
   </si>
   <si>
+    <t>2:40 p.m.</t>
+  </si>
+  <si>
     <t>BRAYAN ANDRÉS LEMUS</t>
   </si>
   <si>
     <t>ALEMÁN</t>
   </si>
   <si>
+    <t>2:48 p.m.</t>
+  </si>
+  <si>
     <t>SAMANTHA CASAS</t>
   </si>
   <si>
@@ -260,12 +299,18 @@
     <t>5:55 a.m.</t>
   </si>
   <si>
+    <t>2:50 p.m.</t>
+  </si>
+  <si>
     <t>JOHANNA CATHERINE QUINTERO</t>
   </si>
   <si>
     <t>INGLÉS 1° Y 2°</t>
   </si>
   <si>
+    <t>2:35 p.m.</t>
+  </si>
+  <si>
     <t>ANDREA PAOLA RICARDO</t>
   </si>
   <si>
@@ -311,6 +356,9 @@
     <t>5:58 a.m.</t>
   </si>
   <si>
+    <t>2:46 p.m.</t>
+  </si>
+  <si>
     <t>NANCY MORALES</t>
   </si>
   <si>
@@ -365,6 +413,9 @@
     <t>SISTEMAS</t>
   </si>
   <si>
+    <t>2:43 p.m.</t>
+  </si>
+  <si>
     <t>YULIANA MORALES</t>
   </si>
   <si>
@@ -380,6 +431,9 @@
     <t>RECTOR</t>
   </si>
   <si>
+    <t>3:05 p.m.</t>
+  </si>
+  <si>
     <t>FYT 17C/ MOTO</t>
   </si>
   <si>
@@ -389,6 +443,9 @@
     <t>COORDINACIÓN ACADÉMICA</t>
   </si>
   <si>
+    <t>2:53 p.m.</t>
+  </si>
+  <si>
     <t>MARCELA PINTO</t>
   </si>
   <si>
@@ -440,6 +497,9 @@
     <t>COORDINACIÓN CONVIVENCIA</t>
   </si>
   <si>
+    <t>2:56 p.m.</t>
+  </si>
+  <si>
     <t>YJE 30F/ MOTO</t>
   </si>
   <si>
@@ -470,6 +530,9 @@
     <t>6:07 a.m.</t>
   </si>
   <si>
+    <t>2:47 p.m.</t>
+  </si>
+  <si>
     <t>MARÍA EUGENIA GARCÍA</t>
   </si>
   <si>
@@ -567,6 +630,51 @@
   </si>
   <si>
     <t>6:37 a.m.</t>
+  </si>
+  <si>
+    <t>TRANSITO CASTILLO</t>
+  </si>
+  <si>
+    <t>7:14 a.m.</t>
+  </si>
+  <si>
+    <t>NUBIA CENAIDA HURTADO</t>
+  </si>
+  <si>
+    <t>7:28 a.m.</t>
+  </si>
+  <si>
+    <t>BERTILDE QUINTERO</t>
+  </si>
+  <si>
+    <t>7:29 a.m.</t>
+  </si>
+  <si>
+    <t>PATRICIA SOTO</t>
+  </si>
+  <si>
+    <t>7:34 a.m.</t>
+  </si>
+  <si>
+    <t>ISABEL MIGUEZ</t>
+  </si>
+  <si>
+    <t>7:50 a.m.</t>
+  </si>
+  <si>
+    <t>LUZ MARINA NEIZA</t>
+  </si>
+  <si>
+    <t>MENSAJERÍA</t>
+  </si>
+  <si>
+    <t>MENSAJERA</t>
+  </si>
+  <si>
+    <t>8:37 a.m.</t>
+  </si>
+  <si>
+    <t>9:55 a.m.</t>
   </si>
   <si>
     <t>LINDA YESENIA HUERTAS</t>
@@ -1027,10 +1135,10 @@
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
   </sheetPr>
-  <dimension ref="A1:I61"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A61" sqref="A61:I61"/>
+      <selection activeCell="A67" sqref="A67:I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1119,7 +1227,9 @@
       <c r="F3" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H3" s="2"/>
       <c r="I3" s="2"/>
     </row>
@@ -1128,21 +1238,23 @@
         <v>9</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" s="3"/>
+        <v>24</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
     </row>
@@ -1151,23 +1263,25 @@
         <v>9</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="3"/>
       <c r="H5" s="2" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I5" s="2"/>
     </row>
@@ -1176,21 +1290,23 @@
         <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G6" s="3"/>
+        <v>34</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>35</v>
+      </c>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
     </row>
@@ -1199,23 +1315,25 @@
         <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G7" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="H7" s="2" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="I7" s="2"/>
     </row>
@@ -1224,7 +1342,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>17</v>
@@ -1232,12 +1350,14 @@
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
       <c r="F8" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G8" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>43</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:9">
@@ -1245,23 +1365,25 @@
         <v>9</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="G9" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H9" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I9" s="2"/>
     </row>
@@ -1270,21 +1392,23 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G10" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
     </row>
@@ -1293,24 +1417,26 @@
         <v>9</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>49</v>
+        <v>56</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="G11" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>40</v>
+      </c>
       <c r="H11" s="2"/>
       <c r="I11" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9">
@@ -1318,19 +1444,21 @@
         <v>9</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>52</v>
+        <v>59</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>54</v>
+        <v>61</v>
       </c>
       <c r="E12" s="2"/>
       <c r="F12" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="2"/>
+        <v>62</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
@@ -1339,21 +1467,23 @@
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="G13" s="2"/>
+        <v>66</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="H13" s="2" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
       <c r="I13" s="2"/>
     </row>
@@ -1362,22 +1492,24 @@
         <v>9</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="C14" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2" t="s">
-        <v>61</v>
+        <v>70</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="G14" s="3"/>
+        <v>71</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="15" spans="1:9">
@@ -1385,19 +1517,21 @@
         <v>9</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>63</v>
+        <v>72</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="E15" s="2"/>
       <c r="F15" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="G15" s="2"/>
+        <v>74</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
     </row>
@@ -1406,19 +1540,21 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2" t="s">
-        <v>67</v>
+        <v>77</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="G16" s="3"/>
+        <v>78</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
     </row>
@@ -1427,17 +1563,17 @@
         <v>9</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>69</v>
+        <v>80</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>71</v>
+        <v>82</v>
       </c>
       <c r="E17" s="2"/>
       <c r="F17" s="2" t="s">
-        <v>68</v>
+        <v>78</v>
       </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -1448,21 +1584,23 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>72</v>
+        <v>83</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>73</v>
+        <v>84</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>74</v>
+        <v>85</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G18" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
     </row>
@@ -1471,19 +1609,21 @@
         <v>9</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D19" s="2"/>
       <c r="E19" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="3"/>
+        <v>86</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
     </row>
@@ -1492,21 +1632,23 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>94</v>
+      </c>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
     </row>
@@ -1515,19 +1657,21 @@
         <v>9</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>81</v>
+        <v>95</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D21" s="2"/>
       <c r="E21" s="2" t="s">
-        <v>82</v>
+        <v>96</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G21" s="3"/>
+        <v>93</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
     </row>
@@ -1536,23 +1680,25 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>83</v>
+        <v>98</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>84</v>
+        <v>99</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G22" s="3"/>
+        <v>101</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>63</v>
+      </c>
       <c r="H22" s="2" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="I22" s="2"/>
     </row>
@@ -1561,21 +1707,23 @@
         <v>9</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G23" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
@@ -1584,21 +1732,23 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="G24" s="3"/>
+        <v>106</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
     </row>
@@ -1607,21 +1757,23 @@
         <v>9</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="G25" s="3"/>
+        <v>112</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
     </row>
@@ -1630,24 +1782,26 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>98</v>
+        <v>114</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>99</v>
+        <v>115</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>100</v>
+        <v>116</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G26" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
     </row>
     <row r="27" spans="1:9">
@@ -1655,21 +1809,23 @@
         <v>9</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>103</v>
+        <v>119</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G27" s="3"/>
+        <v>117</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>54</v>
+      </c>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
     </row>
@@ -1678,21 +1834,23 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D28" s="2"/>
       <c r="E28" s="2" t="s">
-        <v>106</v>
+        <v>122</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="G28" s="3"/>
+        <v>123</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="H28" s="2" t="s">
-        <v>108</v>
+        <v>124</v>
       </c>
       <c r="I28" s="2"/>
     </row>
@@ -1701,21 +1859,23 @@
         <v>9</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>109</v>
+        <v>125</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>110</v>
+        <v>126</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G29" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>113</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
     </row>
@@ -1724,19 +1884,21 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
-        <v>77</v>
+        <v>89</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
     </row>
@@ -1745,19 +1907,21 @@
         <v>9</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>114</v>
+        <v>130</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D31" s="2"/>
       <c r="E31" s="2" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G31" s="3"/>
+        <v>128</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>132</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
     </row>
@@ -1766,21 +1930,23 @@
         <v>9</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G32" s="3"/>
+        <v>135</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
     </row>
@@ -1789,21 +1955,23 @@
         <v>9</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>119</v>
+        <v>136</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>120</v>
+        <v>137</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G33" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>138</v>
+      </c>
       <c r="H33" s="2" t="s">
-        <v>121</v>
+        <v>139</v>
       </c>
       <c r="I33" s="2"/>
     </row>
@@ -1812,19 +1980,21 @@
         <v>9</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>122</v>
+        <v>140</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>123</v>
+        <v>141</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="G34" s="2"/>
+        <v>135</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
     </row>
@@ -1833,21 +2003,23 @@
         <v>9</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>124</v>
+        <v>143</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>125</v>
+        <v>144</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G35" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>87</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
     </row>
@@ -1856,23 +2028,25 @@
         <v>9</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>127</v>
+        <v>146</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>128</v>
+        <v>147</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>129</v>
+        <v>148</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G36" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="H36" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I36" s="2"/>
     </row>
@@ -1881,23 +2055,25 @@
         <v>9</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>130</v>
+        <v>149</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>131</v>
+        <v>150</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>132</v>
+        <v>151</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G37" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="H37" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I37" s="2"/>
     </row>
@@ -1906,23 +2082,25 @@
         <v>9</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>133</v>
+        <v>152</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>134</v>
+        <v>153</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>135</v>
+        <v>154</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="G38" s="3"/>
+        <v>145</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>67</v>
+      </c>
       <c r="H38" s="2" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I38" s="2"/>
     </row>
@@ -1931,21 +2109,23 @@
         <v>9</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>136</v>
+        <v>155</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>137</v>
+        <v>156</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>19</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G39" s="3"/>
+        <v>157</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
     </row>
@@ -1954,21 +2134,23 @@
         <v>9</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>139</v>
+        <v>158</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>53</v>
+        <v>60</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="E40" s="2"/>
       <c r="F40" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G40" s="2"/>
+        <v>157</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>160</v>
+      </c>
       <c r="H40" s="2" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="I40" s="2"/>
     </row>
@@ -1977,17 +2159,17 @@
         <v>9</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="C41" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2" t="s">
-        <v>138</v>
+        <v>157</v>
       </c>
       <c r="G41" s="2"/>
       <c r="H41" s="2"/>
@@ -1998,21 +2180,23 @@
         <v>9</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>146</v>
+        <v>166</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="G42" s="3"/>
+        <v>157</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
     </row>
@@ -2021,21 +2205,23 @@
         <v>9</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>147</v>
+        <v>167</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>148</v>
+        <v>168</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>149</v>
+        <v>169</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G43" s="3"/>
+        <v>170</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>171</v>
+      </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
@@ -2044,17 +2230,17 @@
         <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>151</v>
+        <v>172</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" s="2" t="s">
-        <v>154</v>
+        <v>175</v>
       </c>
       <c r="G44" s="2"/>
       <c r="H44" s="2"/>
@@ -2065,21 +2251,23 @@
         <v>9</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>155</v>
+        <v>176</v>
       </c>
       <c r="C45" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>156</v>
+        <v>177</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>157</v>
+        <v>178</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G45" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
@@ -2088,19 +2276,21 @@
         <v>9</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>158</v>
+        <v>179</v>
       </c>
       <c r="C46" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D46" s="2"/>
       <c r="E46" s="2" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G46" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>79</v>
+      </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
@@ -2109,19 +2299,21 @@
         <v>9</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>160</v>
+        <v>181</v>
       </c>
       <c r="C47" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D47" s="2" t="s">
-        <v>161</v>
+        <v>182</v>
       </c>
       <c r="E47" s="2"/>
       <c r="F47" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G47" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
@@ -2130,19 +2322,21 @@
         <v>9</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>162</v>
+        <v>183</v>
       </c>
       <c r="C48" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D48" s="2"/>
       <c r="E48" s="2" t="s">
-        <v>163</v>
+        <v>184</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="G48" s="3"/>
+        <v>175</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>25</v>
+      </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
@@ -2151,19 +2345,21 @@
         <v>9</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>164</v>
+        <v>185</v>
       </c>
       <c r="C49" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D49" s="2"/>
       <c r="E49" s="2" t="s">
-        <v>165</v>
+        <v>186</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>166</v>
-      </c>
-      <c r="G49" s="3"/>
+        <v>187</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
@@ -2172,7 +2368,7 @@
         <v>9</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>167</v>
+        <v>188</v>
       </c>
       <c r="C50" s="2" t="s">
         <v>17</v>
@@ -2180,9 +2376,11 @@
       <c r="D50" s="2"/>
       <c r="E50" s="2"/>
       <c r="F50" s="2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G50" s="3"/>
+        <v>189</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>48</v>
+      </c>
       <c r="H50" s="2"/>
       <c r="I50" s="2"/>
     </row>
@@ -2191,17 +2389,17 @@
         <v>9</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>169</v>
+        <v>190</v>
       </c>
       <c r="C51" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>170</v>
+        <v>191</v>
       </c>
       <c r="E51" s="2"/>
       <c r="F51" s="2" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="G51" s="2"/>
       <c r="H51" s="2"/>
@@ -2212,17 +2410,17 @@
         <v>9</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>172</v>
+        <v>193</v>
       </c>
       <c r="C52" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>173</v>
+        <v>194</v>
       </c>
       <c r="E52" s="2"/>
       <c r="F52" s="2" t="s">
-        <v>174</v>
+        <v>195</v>
       </c>
       <c r="G52" s="2"/>
       <c r="H52" s="2"/>
@@ -2233,17 +2431,17 @@
         <v>9</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>175</v>
+        <v>196</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>176</v>
+        <v>197</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" s="2" t="s">
-        <v>177</v>
+        <v>198</v>
       </c>
       <c r="G53" s="2"/>
       <c r="H53" s="2"/>
@@ -2254,22 +2452,24 @@
         <v>9</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>178</v>
+        <v>199</v>
       </c>
       <c r="C54" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D54" s="2"/>
       <c r="E54" s="2" t="s">
-        <v>179</v>
+        <v>200</v>
       </c>
       <c r="F54" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="G54" s="3"/>
+        <v>201</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>90</v>
+      </c>
       <c r="H54" s="2"/>
       <c r="I54" s="2" t="s">
-        <v>181</v>
+        <v>202</v>
       </c>
     </row>
     <row r="55" spans="1:9">
@@ -2277,148 +2477,276 @@
         <v>9</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>182</v>
+        <v>203</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>152</v>
+        <v>173</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>153</v>
+        <v>174</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" s="2" t="s">
-        <v>183</v>
+        <v>204</v>
       </c>
       <c r="G55" s="2"/>
       <c r="H55" s="2"/>
       <c r="I55" s="2"/>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D56" s="4"/>
-      <c r="E56" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="F56" s="4"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="4"/>
-      <c r="I56" s="4" t="s">
-        <v>186</v>
-      </c>
+      <c r="A56" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B56" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E56" s="2"/>
+      <c r="F56" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="2"/>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>187</v>
-      </c>
-      <c r="C57" s="4" t="s">
+      <c r="A57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B57" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="C57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E57" s="2"/>
+      <c r="F57" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="G57" s="2"/>
+      <c r="H57" s="2"/>
+      <c r="I57" s="2"/>
+    </row>
+    <row r="58" spans="1:9">
+      <c r="A58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B58" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="C58" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E58" s="2"/>
+      <c r="F58" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="G58" s="2"/>
+      <c r="H58" s="2"/>
+      <c r="I58" s="2"/>
+    </row>
+    <row r="59" spans="1:9">
+      <c r="A59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B59" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C59" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E59" s="2"/>
+      <c r="F59" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="G59" s="2"/>
+      <c r="H59" s="2"/>
+      <c r="I59" s="2"/>
+    </row>
+    <row r="60" spans="1:9">
+      <c r="A60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="C60" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="E60" s="2"/>
+      <c r="F60" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="G60" s="2"/>
+      <c r="H60" s="2"/>
+      <c r="I60" s="2"/>
+    </row>
+    <row r="61" spans="1:9">
+      <c r="A61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B61" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C61" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D61" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E61" s="2"/>
+      <c r="F61" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="H61" s="2"/>
+      <c r="I61" s="2"/>
+    </row>
+    <row r="62" spans="1:9">
+      <c r="A62" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D62" s="4"/>
+      <c r="E62" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="F62" s="4"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9">
+      <c r="A63" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="4" t="s">
-        <v>188</v>
-      </c>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="58" spans="1:9">
-      <c r="A58" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>190</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D58" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="E58" s="4" t="s">
-        <v>192</v>
-      </c>
-      <c r="F58" s="4"/>
-      <c r="G58" s="4"/>
-      <c r="H58" s="4"/>
-      <c r="I58" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="59" spans="1:9">
-      <c r="A59" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>194</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D59" s="4"/>
-      <c r="E59" s="4"/>
-      <c r="F59" s="4"/>
-      <c r="G59" s="4"/>
-      <c r="H59" s="4"/>
-      <c r="I59" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="60" spans="1:9">
-      <c r="A60" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B60" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C60" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="E60" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="F60" s="4"/>
-      <c r="G60" s="4"/>
-      <c r="H60" s="4"/>
-      <c r="I60" s="4" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="61" spans="1:9">
-      <c r="A61" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="B61" s="4" t="s">
-        <v>200</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="D61" s="4"/>
-      <c r="E61" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="F61" s="4"/>
-      <c r="G61" s="4"/>
-      <c r="H61" s="4"/>
-      <c r="I61" s="4" t="s">
-        <v>195</v>
+      <c r="D63" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E63" s="4"/>
+      <c r="F63" s="4"/>
+      <c r="G63" s="4"/>
+      <c r="H63" s="4"/>
+      <c r="I63" s="4" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9">
+      <c r="A64" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D64" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="E64" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="F64" s="4"/>
+      <c r="G64" s="4"/>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9">
+      <c r="A65" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D65" s="4"/>
+      <c r="E65" s="4"/>
+      <c r="F65" s="4"/>
+      <c r="G65" s="4"/>
+      <c r="H65" s="4"/>
+      <c r="I65" s="4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9">
+      <c r="A66" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="E66" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="F66" s="4"/>
+      <c r="G66" s="4"/>
+      <c r="H66" s="4"/>
+      <c r="I66" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9">
+      <c r="A67" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="D67" s="4"/>
+      <c r="E67" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="F67" s="4"/>
+      <c r="G67" s="4"/>
+      <c r="H67" s="4"/>
+      <c r="I67" s="4" t="s">
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>